<commit_message>
Implement premade menu from data.js
</commit_message>
<xml_diff>
--- a/src/options.xlsx
+++ b/src/options.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2021158\OneDrive - Appleby College\Documents\GitHub\trailmix-order\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2021158\OneDrive - Appleby College\S2\IB\Shared Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21E7D5B-D1FD-463C-9E21-F64D1D7F1920}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DEFDD4-5EFE-4CE4-A2D2-F887B6F9C870}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24250" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24250" windowHeight="16860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Options" sheetId="1" r:id="rId1"/>
-    <sheet name="Defaults" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Premade" sheetId="3" r:id="rId2"/>
+    <sheet name="Defaults" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,19 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Bulk Barn ID</t>
-  </si>
-  <si>
-    <t>Price pre 100g</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
   <si>
     <t>Flavouring</t>
   </si>
@@ -118,18 +107,9 @@
     <t>BBQ Seasoning</t>
   </si>
   <si>
-    <t>Density (g/cm3)</t>
-  </si>
-  <si>
-    <t>Cents per cm3</t>
-  </si>
-  <si>
     <t>Cinnamon Sugar</t>
   </si>
   <si>
-    <t>Link</t>
-  </si>
-  <si>
     <t>https://www.bulkbarn.ca/en/Products/All/Bbq-Ringolos-50</t>
   </si>
   <si>
@@ -182,6 +162,39 @@
   </si>
   <si>
     <t>https://www.bulkbarn.ca/en/Products/All/MandMS-Plain-Chocolate-Candies-620</t>
+  </si>
+  <si>
+    <t>Example Mix 1</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>imageLink</t>
+  </si>
+  <si>
+    <t>https://nuts.com/images/rackcdn/ed910ae2d60f0d25bcb8-80550f96b5feb12604f4f720bfefb46d.ssl.cf1.rackcdn.com/8002_HealthyTrailMix-p92BoPXo-zoom.jpg</t>
+  </si>
+  <si>
+    <t>cents_per_cm3</t>
+  </si>
+  <si>
+    <t>density</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>price_per_100g</t>
+  </si>
+  <si>
+    <t>bbid</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -209,7 +222,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,6 +244,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,7 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -288,6 +307,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -569,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -587,35 +607,38 @@
     <col min="8" max="8" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -624,7 +647,7 @@
         <v>1.08</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F2" s="6">
         <v>0.14000000000000001</v>
@@ -634,12 +657,12 @@
         <v>0.15120000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C3">
         <v>58</v>
@@ -648,7 +671,7 @@
         <v>0.51</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F3" s="10">
         <v>0.51</v>
@@ -658,12 +681,12 @@
         <v>0.2601</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C4">
         <v>23</v>
@@ -672,7 +695,7 @@
         <v>0.92</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F4" s="5">
         <v>0.38</v>
@@ -682,12 +705,12 @@
         <v>0.34960000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>938</v>
@@ -696,7 +719,7 @@
         <v>1.05</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F5" s="5">
         <v>0.41</v>
@@ -706,12 +729,12 @@
         <v>0.43049999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C6">
         <v>135</v>
@@ -720,7 +743,7 @@
         <v>0.85</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F6" s="5">
         <v>0.54</v>
@@ -730,12 +753,12 @@
         <v>0.45900000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C7">
         <v>108</v>
@@ -744,7 +767,7 @@
         <v>0.76</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F7" s="11">
         <v>0.64</v>
@@ -754,12 +777,12 @@
         <v>0.4864</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>1700</v>
@@ -768,7 +791,7 @@
         <v>0.72</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F8" s="5">
         <v>0.68</v>
@@ -778,12 +801,12 @@
         <v>0.48960000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C9">
         <v>2447</v>
@@ -792,7 +815,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="E9" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F9" s="5">
         <v>0.51</v>
@@ -802,12 +825,12 @@
         <v>0.58649999999999991</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C10">
         <v>1729</v>
@@ -816,7 +839,7 @@
         <v>1.99</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F10" s="11">
         <v>0.34</v>
@@ -826,12 +849,12 @@
         <v>0.67660000000000009</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C11">
         <v>859</v>
@@ -840,7 +863,7 @@
         <v>1.33</v>
       </c>
       <c r="E11" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F11" s="5">
         <v>0.53</v>
@@ -850,12 +873,12 @@
         <v>0.70490000000000008</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C12">
         <v>3274</v>
@@ -864,7 +887,7 @@
         <v>1.97</v>
       </c>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F12" s="5">
         <v>0.41</v>
@@ -874,12 +897,12 @@
         <v>0.80769999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C13">
         <v>1794</v>
@@ -888,7 +911,7 @@
         <v>1.25</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F13" s="5">
         <v>0.68</v>
@@ -898,12 +921,12 @@
         <v>0.85000000000000009</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C14">
         <v>1794</v>
@@ -912,7 +935,7 @@
         <v>0.99</v>
       </c>
       <c r="E14" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F14" s="5">
         <v>1.01</v>
@@ -922,12 +945,12 @@
         <v>0.99990000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C15">
         <v>1773</v>
@@ -936,7 +959,7 @@
         <v>2.88</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F15" s="5">
         <v>0.47</v>
@@ -946,12 +969,12 @@
         <v>1.3535999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C16">
         <v>28</v>
@@ -960,7 +983,7 @@
         <v>2.0499999999999998</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F16" s="5">
         <v>0.68</v>
@@ -972,10 +995,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C17">
         <v>118</v>
@@ -984,7 +1007,7 @@
         <v>2.56</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F17" s="5">
         <v>0.62</v>
@@ -996,10 +1019,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C18">
         <v>113</v>
@@ -1008,7 +1031,7 @@
         <v>3.09</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F18" s="9">
         <v>0.57999999999999996</v>
@@ -1020,10 +1043,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C19">
         <v>620</v>
@@ -1032,7 +1055,7 @@
         <v>2.4700000000000002</v>
       </c>
       <c r="E19" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F19" s="5">
         <v>0.86</v>
@@ -1085,7 +1108,7 @@
           <x14:formula1>
             <xm:f>Defaults!$A$1:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D20:D1048576 E1:E19</xm:sqref>
+          <xm:sqref>D20:D1048576 E2:E19</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1094,6 +1117,115 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{010AEDD3-8629-41EE-A299-7FEE3E2E84D9}">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A5687E8-A2E5-423B-95B3-28ECB0F8801A}">
   <dimension ref="A1:A6"/>
   <sheetViews>
@@ -1105,32 +1237,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add in category and limit support, restructure to modify state of order
</commit_message>
<xml_diff>
--- a/src/options.xlsx
+++ b/src/options.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2021158\OneDrive - Appleby College\S2\IB\Shared Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DEFDD4-5EFE-4CE4-A2D2-F887B6F9C870}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EDBC6B0-831D-430C-8F0B-0504E99EBC80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24250" windowHeight="16860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24250" windowHeight="16860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Options" sheetId="1" r:id="rId1"/>
     <sheet name="Premade" sheetId="3" r:id="rId2"/>
-    <sheet name="Defaults" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="Defaults" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="57">
   <si>
     <t>Flavouring</t>
   </si>
@@ -164,18 +164,12 @@
     <t>https://www.bulkbarn.ca/en/Products/All/MandMS-Plain-Chocolate-Candies-620</t>
   </si>
   <si>
-    <t>Example Mix 1</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
     <t>imageLink</t>
   </si>
   <si>
-    <t>https://nuts.com/images/rackcdn/ed910ae2d60f0d25bcb8-80550f96b5feb12604f4f720bfefb46d.ssl.cf1.rackcdn.com/8002_HealthyTrailMix-p92BoPXo-zoom.jpg</t>
-  </si>
-  <si>
     <t>cents_per_cm3</t>
   </si>
   <si>
@@ -195,6 +189,24 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>Keto Mix</t>
+  </si>
+  <si>
+    <t>Sweet Lovers</t>
+  </si>
+  <si>
+    <t>Classic Mix</t>
+  </si>
+  <si>
+    <t>Crunchy Mix</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>Limit</t>
   </si>
 </sst>
 </file>
@@ -222,7 +234,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,6 +262,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,7 +309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -308,6 +326,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -592,7 +611,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -609,28 +628,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1106,7 +1125,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C4C03165-4AFD-4EE5-937F-7552039363B4}">
           <x14:formula1>
-            <xm:f>Defaults!$A$1:$A$6</xm:f>
+            <xm:f>Defaults!$A$2:$A$6</xm:f>
           </x14:formula1>
           <xm:sqref>D20:D1048576 E2:E19</xm:sqref>
         </x14:dataValidation>
@@ -1118,10 +1137,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{010AEDD3-8629-41EE-A299-7FEE3E2E84D9}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1131,7 +1150,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>18</v>
@@ -1188,36 +1207,102 @@
         <v>15</v>
       </c>
       <c r="T1" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P2" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>42</v>
       </c>
       <c r="R2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T2" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R3" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
+      <c r="S4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1227,42 +1312,71 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A5687E8-A2E5-423B-95B3-28ECB0F8801A}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add in accurate pricing system
</commit_message>
<xml_diff>
--- a/src/options.xlsx
+++ b/src/options.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2021158\OneDrive - Appleby College\S2\IB\Shared Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E4FF5D-50F2-4872-A27A-BBF5661E64C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF88EB8-C5E3-413E-91D7-0271B5486710}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24250" windowHeight="16860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="62">
   <si>
     <t>Flavouring</t>
   </si>
@@ -107,9 +107,6 @@
     <t>BBQ Seasoning</t>
   </si>
   <si>
-    <t>Cinnamon Sugar</t>
-  </si>
-  <si>
     <t>https://www.bulkbarn.ca/en/Products/All/Bbq-Ringolos-50</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
     <t>https://www.bulkbarn.ca/en/Products/All/Dried-Mango-Slices-1729</t>
   </si>
   <si>
-    <t>https://www.bulkbarn.ca/en/Products/All/Cinnamon-Sugar-859</t>
-  </si>
-  <si>
     <t>https://www.bulkbarn.ca/en/Products/All/Marshmallow-Hearts</t>
   </si>
   <si>
@@ -207,6 +201,27 @@
   </si>
   <si>
     <t xml:space="preserve">Sweet Lovers Mix </t>
+  </si>
+  <si>
+    <t>https://www.bulkbarn.ca/en/Products/All/Cinnamon-Ground-913</t>
+  </si>
+  <si>
+    <t>Ground Cinnamon</t>
+  </si>
+  <si>
+    <t>value_served</t>
+  </si>
+  <si>
+    <t>mass_served</t>
+  </si>
+  <si>
+    <t>official_cost</t>
+  </si>
+  <si>
+    <t>as needed</t>
+  </si>
+  <si>
+    <t>price</t>
   </si>
 </sst>
 </file>
@@ -608,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -622,42 +637,53 @@
     <col min="4" max="4" width="11.26953125" customWidth="1"/>
     <col min="5" max="5" width="15.26953125" customWidth="1"/>
     <col min="6" max="6" width="15.08984375" customWidth="1"/>
-    <col min="7" max="7" width="12.08984375" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" customWidth="1"/>
     <col min="8" max="8" width="17.453125" customWidth="1"/>
+    <col min="9" max="9" width="16.90625" customWidth="1"/>
+    <col min="10" max="10" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -675,13 +701,23 @@
         <f t="shared" ref="G2:G19" si="0">(D2*F2)</f>
         <v>0.15120000000000003</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2" s="7">
+        <f>100/(D2/H2)</f>
+        <v>46.296296296296291</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>58</v>
@@ -699,13 +735,23 @@
         <f t="shared" si="0"/>
         <v>0.2601</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H3">
+        <v>0.5</v>
+      </c>
+      <c r="I3" s="7">
+        <f t="shared" ref="I3:I19" si="1">100/(D3/H3)</f>
+        <v>98.039215686274503</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4">
         <v>23</v>
@@ -723,13 +769,23 @@
         <f t="shared" si="0"/>
         <v>0.34960000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H4">
+        <v>0.5</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="1"/>
+        <v>54.347826086956516</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <v>938</v>
@@ -747,13 +803,22 @@
         <f t="shared" si="0"/>
         <v>0.43049999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H5">
+        <v>0.5</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6">
         <v>135</v>
@@ -771,13 +836,23 @@
         <f t="shared" si="0"/>
         <v>0.45900000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H6">
+        <v>0.5</v>
+      </c>
+      <c r="I6" s="7">
+        <f t="shared" si="1"/>
+        <v>58.82352941176471</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7">
         <v>108</v>
@@ -795,13 +870,23 @@
         <f t="shared" si="0"/>
         <v>0.4864</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H7">
+        <v>0.5</v>
+      </c>
+      <c r="I7" s="7">
+        <f t="shared" si="1"/>
+        <v>65.78947368421052</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8">
         <v>1700</v>
@@ -819,13 +904,23 @@
         <f t="shared" si="0"/>
         <v>0.48960000000000004</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H8">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="7">
+        <f t="shared" si="1"/>
+        <v>69.444444444444443</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <v>2447</v>
@@ -843,13 +938,22 @@
         <f t="shared" si="0"/>
         <v>0.58649999999999991</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H9">
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10">
         <v>1729</v>
@@ -867,16 +971,26 @@
         <f t="shared" si="0"/>
         <v>0.67660000000000009</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H10">
+        <v>0.5</v>
+      </c>
+      <c r="I10" s="7">
+        <f t="shared" si="1"/>
+        <v>25.125628140703519</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
+        <v>56</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="C11">
-        <v>859</v>
+        <v>913</v>
       </c>
       <c r="D11" s="4">
         <v>1.33</v>
@@ -891,13 +1005,22 @@
         <f t="shared" si="0"/>
         <v>0.70490000000000008</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H11">
+        <v>0.5</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>3274</v>
@@ -915,13 +1038,23 @@
         <f t="shared" si="0"/>
         <v>0.80769999999999997</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H12">
+        <v>0.5</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="1"/>
+        <v>25.380710659898476</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13">
         <v>1794</v>
@@ -939,13 +1072,23 @@
         <f t="shared" si="0"/>
         <v>0.85000000000000009</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H13">
+        <v>0.5</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C14">
         <v>1794</v>
@@ -963,13 +1106,23 @@
         <f t="shared" si="0"/>
         <v>0.99990000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H14">
+        <v>0.5</v>
+      </c>
+      <c r="I14" s="7">
+        <f t="shared" si="1"/>
+        <v>50.505050505050505</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15">
         <v>1773</v>
@@ -987,13 +1140,23 @@
         <f t="shared" si="0"/>
         <v>1.3535999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H15">
+        <v>0.5</v>
+      </c>
+      <c r="I15" s="7">
+        <f t="shared" si="1"/>
+        <v>17.361111111111111</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C16">
         <v>28</v>
@@ -1011,13 +1174,23 @@
         <f t="shared" si="0"/>
         <v>1.3939999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H16">
+        <v>0.5</v>
+      </c>
+      <c r="I16" s="7">
+        <f t="shared" si="1"/>
+        <v>24.390243902439025</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C17">
         <v>118</v>
@@ -1035,13 +1208,23 @@
         <f t="shared" si="0"/>
         <v>1.5871999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H17">
+        <v>0.5</v>
+      </c>
+      <c r="I17" s="7">
+        <f t="shared" si="1"/>
+        <v>19.53125</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18">
         <v>113</v>
@@ -1059,13 +1242,23 @@
         <f t="shared" si="0"/>
         <v>1.7921999999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H18">
+        <v>0.5</v>
+      </c>
+      <c r="I18" s="7">
+        <f t="shared" si="1"/>
+        <v>16.181229773462785</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19">
         <v>620</v>
@@ -1082,6 +1275,16 @@
       <c r="G19" s="8">
         <f t="shared" si="0"/>
         <v>2.1242000000000001</v>
+      </c>
+      <c r="H19">
+        <v>0.5</v>
+      </c>
+      <c r="I19" s="7">
+        <f t="shared" si="1"/>
+        <v>20.242914979757085</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1137,10 +1340,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{010AEDD3-8629-41EE-A299-7FEE3E2E84D9}">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1148,9 +1351,9 @@
     <col min="1" max="1" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>18</v>
@@ -1180,7 +1383,7 @@
         <v>10</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>16</v>
@@ -1207,102 +1410,114 @@
         <v>15</v>
       </c>
       <c r="T1" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="R2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="T2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="R3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="T3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="T4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="N5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P5" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="T5">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1315,7 +1530,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1325,10 +1540,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Rewrite of extractData.js using more developed library
</commit_message>
<xml_diff>
--- a/src/options.xlsx
+++ b/src/options.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2021158\OneDrive - Appleby College\S2\IB\Shared Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33099C9F-6A6B-4E27-9075-0312D2B58177}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A95C128-AEA2-45E4-AB63-D729D73E04B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24250" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="63">
   <si>
     <t>Flavouring</t>
   </si>
@@ -122,9 +122,6 @@
     <t>https://www.bulkbarn.ca/en/Products/All/Sunflower-Seeds-Hulled-Roasted-and-Salted-135</t>
   </si>
   <si>
-    <t>https://www.bulkbarn.ca/en/Products/All/Peanuts-Dry-Roasted-and-Seasoned-108</t>
-  </si>
-  <si>
     <t>https://www.bulkbarn.ca/en/Products/All/Sultana-Raisins-Seedless-1700</t>
   </si>
   <si>
@@ -216,6 +213,15 @@
   </si>
   <si>
     <t>official_cost</t>
+  </si>
+  <si>
+    <t>order_servings</t>
+  </si>
+  <si>
+    <t>order_mass</t>
+  </si>
+  <si>
+    <t>https://www.bulkbarn.ca/en/Products/All/Peanuts-Raw-and-Blanched-102</t>
   </si>
   <si>
     <t>price</t>
@@ -620,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -638,45 +644,53 @@
     <col min="8" max="8" width="17.453125" customWidth="1"/>
     <col min="9" max="9" width="16.90625" customWidth="1"/>
     <col min="10" max="10" width="14.54296875" customWidth="1"/>
-    <col min="11" max="11" width="10.81640625" customWidth="1"/>
+    <col min="11" max="11" width="11.6328125" customWidth="1"/>
+    <col min="12" max="12" width="13.6328125" customWidth="1"/>
+    <col min="13" max="13" width="11.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M1" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>18</v>
       </c>
@@ -702,14 +716,22 @@
       <c r="H2">
         <v>0.5</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" s="7">
-        <v>46.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="7">
+        <f t="shared" ref="J2:J19" si="1">100/(D2/H2)</f>
+        <v>46.296296296296291</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ref="K2:K19" si="2">L2*J2</f>
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>17</v>
       </c>
@@ -735,14 +757,22 @@
       <c r="H3">
         <v>0.5</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3" s="7">
-        <v>98.04</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7">
+        <f t="shared" si="1"/>
+        <v>98.039215686274503</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
@@ -768,14 +798,22 @@
       <c r="H4">
         <v>0.5</v>
       </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4" s="7">
-        <v>54.35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="1"/>
+        <v>54.347826086956516</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>22</v>
       </c>
@@ -801,14 +839,22 @@
       <c r="H5">
         <v>0.5</v>
       </c>
-      <c r="J5">
-        <v>0.5</v>
-      </c>
-      <c r="K5" s="7">
-        <v>47.62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" si="1"/>
+        <v>47.61904761904762</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>20</v>
       </c>
@@ -834,85 +880,109 @@
       <c r="H6">
         <v>0.5</v>
       </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6" s="7">
-        <v>58.82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="1"/>
+        <v>58.82352941176471</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
       </c>
       <c r="C7">
-        <v>108</v>
+        <v>1700</v>
       </c>
       <c r="D7" s="1">
-        <v>0.76</v>
+        <v>0.72</v>
       </c>
       <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="11">
-        <v>0.64</v>
+        <v>3</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.68</v>
       </c>
       <c r="G7" s="7">
         <f t="shared" si="0"/>
-        <v>0.4864</v>
+        <v>0.48960000000000004</v>
       </c>
       <c r="H7">
         <v>0.5</v>
       </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7" s="7">
-        <v>65.790000000000006</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="1"/>
+        <v>69.444444444444443</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="C8">
-        <v>1700</v>
+        <v>101</v>
       </c>
       <c r="D8" s="1">
-        <v>0.72</v>
+        <v>0.84</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0.68</v>
+        <v>4</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0.64</v>
       </c>
       <c r="G8" s="7">
         <f t="shared" si="0"/>
-        <v>0.48960000000000004</v>
+        <v>0.53759999999999997</v>
       </c>
       <c r="H8">
         <v>0.5</v>
       </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8" s="7">
-        <v>69.44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" si="1"/>
+        <v>59.523809523809526</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9">
         <v>2447</v>
@@ -933,19 +1003,27 @@
       <c r="H9">
         <v>0.5</v>
       </c>
-      <c r="J9">
-        <v>0.5</v>
-      </c>
-      <c r="K9" s="7">
-        <v>43.48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9" s="7">
+        <f t="shared" si="1"/>
+        <v>43.478260869565219</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>1729</v>
@@ -966,19 +1044,27 @@
       <c r="H10">
         <v>0.5</v>
       </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10" s="7">
-        <v>25.13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="1"/>
+        <v>25.125628140703519</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C11">
         <v>913</v>
@@ -999,19 +1085,27 @@
       <c r="H11">
         <v>0.5</v>
       </c>
-      <c r="J11">
-        <v>0.5</v>
-      </c>
-      <c r="K11" s="7">
-        <v>37.590000000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11" s="7">
+        <f t="shared" si="1"/>
+        <v>37.593984962406012</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12">
         <v>3274</v>
@@ -1032,19 +1126,27 @@
       <c r="H12">
         <v>0.5</v>
       </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12" s="7">
-        <v>25.38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="1"/>
+        <v>25.380710659898476</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>1794</v>
@@ -1065,19 +1167,27 @@
       <c r="H13">
         <v>0.5</v>
       </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13" s="7">
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14">
         <v>1794</v>
@@ -1098,19 +1208,27 @@
       <c r="H14">
         <v>0.5</v>
       </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="K14" s="7">
-        <v>50.51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="1"/>
+        <v>50.505050505050505</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15">
         <v>1773</v>
@@ -1131,19 +1249,27 @@
       <c r="H15">
         <v>0.5</v>
       </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="K15" s="7">
-        <v>17.36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15" s="7">
+        <f t="shared" si="1"/>
+        <v>17.361111111111111</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16">
         <v>28</v>
@@ -1164,19 +1290,27 @@
       <c r="H16">
         <v>0.5</v>
       </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-      <c r="K16" s="7">
-        <v>24.39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16" s="7">
+        <f t="shared" si="1"/>
+        <v>24.390243902439025</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17">
         <v>118</v>
@@ -1197,19 +1331,27 @@
       <c r="H17">
         <v>0.5</v>
       </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="K17" s="7">
-        <v>19.53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" si="1"/>
+        <v>19.53125</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18">
         <v>113</v>
@@ -1230,19 +1372,27 @@
       <c r="H18">
         <v>0.5</v>
       </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
-      <c r="K18" s="7">
-        <v>16.18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18" s="7">
+        <f t="shared" si="1"/>
+        <v>16.181229773462785</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19">
         <v>620</v>
@@ -1263,14 +1413,25 @@
       <c r="H19">
         <v>0.5</v>
       </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
-      <c r="K19" s="7">
-        <v>20.239999999999998</v>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19" s="7">
+        <f t="shared" si="1"/>
+        <v>20.242914979757085</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M19">
+    <sortCondition ref="G2:G19"/>
+  </sortState>
   <conditionalFormatting sqref="G2:G19">
     <cfRule type="colorScale" priority="3">
       <colorScale>
@@ -1285,12 +1446,12 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" display="https://www.aqua-calc.com/page/density-table/substance/banana-blank-chips-coma-and-blank-upc-column--blank-021140022707" xr:uid="{781AF3CE-1674-472E-8935-24CE230E9DE5}"/>
-    <hyperlink ref="F7" r:id="rId2" display="https://www.aqua-calc.com/page/density-table/substance/peanuts-coma-and-blank-shelled" xr:uid="{F64E8304-87E4-40AE-B2BE-6258F6D820B6}"/>
+    <hyperlink ref="F8" r:id="rId2" display="https://www.aqua-calc.com/page/density-table/substance/peanuts-coma-and-blank-shelled" xr:uid="{F64E8304-87E4-40AE-B2BE-6258F6D820B6}"/>
     <hyperlink ref="F18" r:id="rId3" display="https://www.aqua-calc.com/page/density-table/substance/nuts-coma-and-blank-cashew-blank-nuts-coma-and-blank-dry-blank-roasted-coma-and-blank-without-blank-salt-blank-added" xr:uid="{C9416A82-7DF0-491F-ABB1-C296B894993C}"/>
     <hyperlink ref="F17" r:id="rId4" display="https://www.aqua-calc.com/page/density-table/substance/nuts-coma-and-blank-almonds-coma-and-blank-blanched" xr:uid="{B27F59D6-F4E6-49D3-ACEB-A96739AB25ED}"/>
     <hyperlink ref="F15" r:id="rId5" display="https://www.aqua-calc.com/page/density-table/substance/chopped-blank-walnuts-coma-and-blank-upc-column--blank-085239521106" xr:uid="{32F80FD1-D4C1-483C-9022-37489292185B}"/>
     <hyperlink ref="F10" r:id="rId6" display="https://www.aqua-calc.com/page/density-table/substance/dried-blank-mango-coma-and-blank-upc-column--blank-07789043536" xr:uid="{691B87C7-A2AE-4B66-ADD2-18F2EC25AB4E}"/>
-    <hyperlink ref="F8" r:id="rId7" display="https://www.aqua-calc.com/page/density-table/substance/sultana-blank-raisins-coma-and-blank-upc-column--blank-064777812860" xr:uid="{AAC64073-E587-400E-A88D-4943C86C70BF}"/>
+    <hyperlink ref="F7" r:id="rId7" display="https://www.aqua-calc.com/page/density-table/substance/sultana-blank-raisins-coma-and-blank-upc-column--blank-064777812860" xr:uid="{AAC64073-E587-400E-A88D-4943C86C70BF}"/>
     <hyperlink ref="F13" r:id="rId8" display="https://www.aqua-calc.com/page/density-table/substance/dried-blank-cranberries-coma-and-blank-upc-column--blank-070253730535" xr:uid="{4A213918-DDA9-4EB7-AB42-E491AD4F7E29}"/>
     <hyperlink ref="F14" r:id="rId9" display="https://www.aqua-calc.com/page/density-table/substance/chocolate-blank-chips-coma-and-blank-upc-column--blank-032797006521" xr:uid="{BC37C66D-4FBE-43A8-906A-E7ED8A659D8A}"/>
     <hyperlink ref="F19" r:id="rId10" display="https://www.aqua-calc.com/page/density-table/substance/candies-coma-and-blank-mars-blank-snackfood-blank-us-coma-and-blank-m-blank-and-blank-m-quote-s-blank-peanut-blank-butter-blank-chocolate-blank-candies" xr:uid="{1CA35834-A899-4A7B-92C4-2AAB88207E91}"/>
@@ -1302,10 +1463,9 @@
     <hyperlink ref="F11" r:id="rId16" display="https://www.aqua-calc.com/page/density-table/substance/spices-coma-and-blank-cinnamon-coma-and-blank-ground" xr:uid="{5997A6D7-280D-4232-B9E9-A092F1FF1F92}"/>
     <hyperlink ref="F9" r:id="rId17" display="https://www.aqua-calc.com/page/density-table/substance/sweetened-blank-coconut-blank-flakes-coma-and-blank-upc-column--blank-041268113903" xr:uid="{0FC0609E-7C78-4EA0-BCDD-C69558E6BCC5}"/>
     <hyperlink ref="F5" r:id="rId18" display="https://www.aqua-calc.com/page/density-table/substance/barbecue-blank-seasoning-blank-and-blank-rub-coma-and-blank-upc-column--blank-780778107506" xr:uid="{7091F06C-375D-4783-BCA2-89A624AB9A88}"/>
-    <hyperlink ref="D11" r:id="rId19" display="https://www.walmart.ca/en/ip/great-value-ground-cinnamon/6000196207716" xr:uid="{EBFA6B3A-4BB4-4BE2-9268-9280484FBB43}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1326,7 +1486,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1336,7 +1496,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>18</v>
@@ -1366,7 +1526,7 @@
         <v>10</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>16</v>
@@ -1393,33 +1553,33 @@
         <v>15</v>
       </c>
       <c r="T1" s="13" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="U1" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T2">
         <v>6</v>
@@ -1427,25 +1587,25 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T3">
         <v>6</v>
@@ -1453,25 +1613,25 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T4">
         <v>6</v>
@@ -1479,25 +1639,25 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T5">
         <v>6</v>
@@ -1523,10 +1683,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>51</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Remove wieghts for flavorings
</commit_message>
<xml_diff>
--- a/src/options.xlsx
+++ b/src/options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://applebycollege-my.sharepoint.com/personal/2021158_appleby_on_ca/Documents/S2/IB/Shared Folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{D26C5D6C-6008-4239-8AEB-A7AEF841C2F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9C51944F-DD70-40CD-A309-5C3E4C4BDDD3}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{D26C5D6C-6008-4239-8AEB-A7AEF841C2F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3919F133-03C9-479A-B125-BF7627225454}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24250" windowHeight="16860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24250" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Options" sheetId="1" r:id="rId1"/>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -808,8 +808,7 @@
         <v>0.5</v>
       </c>
       <c r="K5" s="7">
-        <f t="shared" si="1"/>
-        <v>47.61904761904762</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -944,8 +943,7 @@
         <v>0.5</v>
       </c>
       <c r="K9" s="7">
-        <f t="shared" si="1"/>
-        <v>43.478260869565219</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -1012,8 +1010,7 @@
         <v>0.5</v>
       </c>
       <c r="K11" s="7">
-        <f t="shared" si="1"/>
-        <v>37.593984962406012</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -1343,7 +1340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{010AEDD3-8629-41EE-A299-7FEE3E2E84D9}">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add total mass counter after price
</commit_message>
<xml_diff>
--- a/src/options.xlsx
+++ b/src/options.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://applebycollege-my.sharepoint.com/personal/2021158_appleby_on_ca/Documents/S2/IB/Shared Folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{D26C5D6C-6008-4239-8AEB-A7AEF841C2F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3919F133-03C9-479A-B125-BF7627225454}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="8_{D26C5D6C-6008-4239-8AEB-A7AEF841C2F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{181BC189-68BC-4C61-8B07-55EFCC32AABD}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24250" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="64">
   <si>
     <t>Flavouring</t>
   </si>
@@ -219,6 +219,15 @@
   </si>
   <si>
     <t>price</t>
+  </si>
+  <si>
+    <t>amount_buy</t>
+  </si>
+  <si>
+    <t>mass_buy</t>
+  </si>
+  <si>
+    <t>order_cost</t>
   </si>
 </sst>
 </file>
@@ -246,7 +255,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,6 +289,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,7 +336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -339,6 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -620,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -639,9 +655,12 @@
     <col min="9" max="9" width="16.90625" customWidth="1"/>
     <col min="10" max="10" width="14.54296875" customWidth="1"/>
     <col min="11" max="11" width="11.6328125" customWidth="1"/>
+    <col min="12" max="12" width="14.26953125" customWidth="1"/>
+    <col min="13" max="13" width="13.6328125" customWidth="1"/>
+    <col min="14" max="14" width="10.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>48</v>
       </c>
@@ -675,8 +694,17 @@
       <c r="K1" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>18</v>
       </c>
@@ -709,8 +737,12 @@
         <f t="shared" ref="K2:K19" si="1">100/(D2/H2)</f>
         <v>46.296296296296291</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M2">
+        <f t="shared" ref="M2:M17" si="2">L2*K2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>17</v>
       </c>
@@ -743,8 +775,12 @@
         <f t="shared" si="1"/>
         <v>98.039215686274503</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
@@ -777,8 +813,12 @@
         <f t="shared" si="1"/>
         <v>54.347826086956516</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>22</v>
       </c>
@@ -810,8 +850,12 @@
       <c r="K5" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>20</v>
       </c>
@@ -844,8 +888,12 @@
         <f t="shared" si="1"/>
         <v>58.82352941176471</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
@@ -878,8 +926,15 @@
         <f t="shared" si="1"/>
         <v>65.78947368421052</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L7">
+        <v>32</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>2105.2631578947367</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
@@ -912,8 +967,15 @@
         <f t="shared" si="1"/>
         <v>69.444444444444443</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L8">
+        <v>20</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>1388.8888888888889</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>21</v>
       </c>
@@ -945,8 +1007,12 @@
       <c r="K9" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>10</v>
       </c>
@@ -979,8 +1045,15 @@
         <f t="shared" si="1"/>
         <v>25.125628140703519</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L10">
+        <v>36</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="2"/>
+        <v>904.52261306532671</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>56</v>
       </c>
@@ -1012,8 +1085,12 @@
       <c r="K11" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>16</v>
       </c>
@@ -1046,8 +1123,12 @@
         <f t="shared" si="1"/>
         <v>25.380710659898476</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>13</v>
       </c>
@@ -1080,8 +1161,15 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L13">
+        <v>29</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="2"/>
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>14</v>
       </c>
@@ -1114,8 +1202,12 @@
         <f t="shared" si="1"/>
         <v>50.505050505050505</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>9</v>
       </c>
@@ -1148,8 +1240,15 @@
         <f t="shared" si="1"/>
         <v>17.361111111111111</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L15">
+        <v>20</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="2"/>
+        <v>347.22222222222223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>19</v>
       </c>
@@ -1182,8 +1281,12 @@
         <f t="shared" si="1"/>
         <v>24.390243902439025</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>8</v>
       </c>
@@ -1216,8 +1319,15 @@
         <f t="shared" si="1"/>
         <v>19.53125</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L17">
+        <v>34</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="2"/>
+        <v>664.0625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>7</v>
       </c>
@@ -1250,8 +1360,15 @@
         <f t="shared" si="1"/>
         <v>16.181229773462785</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L18">
+        <v>34</v>
+      </c>
+      <c r="M18">
+        <f>L18*K18</f>
+        <v>550.16181229773474</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>15</v>
       </c>
@@ -1283,6 +1400,16 @@
       <c r="K19" s="7">
         <f t="shared" si="1"/>
         <v>20.242914979757085</v>
+      </c>
+      <c r="M19">
+        <f>L19*K19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M20" s="15">
+        <f>SUM(M2:M19)</f>
+        <v>7120.1211943689086</v>
       </c>
     </row>
   </sheetData>
@@ -1341,7 +1468,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1528,12 +1655,13 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.7265625" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1549,7 +1677,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add in images from bulk barn
</commit_message>
<xml_diff>
--- a/src/options.xlsx
+++ b/src/options.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://applebycollege-my.sharepoint.com/personal/2021158_appleby_on_ca/Documents/S2/IB/Shared Folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="8_{D26C5D6C-6008-4239-8AEB-A7AEF841C2F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{181BC189-68BC-4C61-8B07-55EFCC32AABD}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="8_{D26C5D6C-6008-4239-8AEB-A7AEF841C2F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E143CE5D-6F30-4058-97F6-E988F63E0FD0}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24250" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="64">
   <si>
     <t>Flavouring</t>
   </si>
@@ -255,7 +255,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,12 +289,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -336,7 +330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -354,7 +348,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -636,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -652,15 +645,14 @@
     <col min="6" max="6" width="15.08984375" customWidth="1"/>
     <col min="7" max="7" width="14.7265625" customWidth="1"/>
     <col min="8" max="8" width="17.453125" customWidth="1"/>
-    <col min="9" max="9" width="16.90625" customWidth="1"/>
-    <col min="10" max="10" width="14.54296875" customWidth="1"/>
-    <col min="11" max="11" width="11.6328125" customWidth="1"/>
-    <col min="12" max="12" width="14.26953125" customWidth="1"/>
-    <col min="13" max="13" width="13.6328125" customWidth="1"/>
-    <col min="14" max="14" width="10.08984375" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" customWidth="1"/>
+    <col min="10" max="10" width="11.6328125" customWidth="1"/>
+    <col min="11" max="11" width="14.26953125" customWidth="1"/>
+    <col min="12" max="12" width="13.6328125" customWidth="1"/>
+    <col min="13" max="13" width="10.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>48</v>
       </c>
@@ -686,25 +678,22 @@
         <v>57</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>18</v>
       </c>
@@ -730,19 +719,26 @@
       <c r="H2">
         <v>0.5</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" s="7">
-        <f t="shared" ref="K2:K19" si="1">100/(D2/H2)</f>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="7">
+        <f>100/(D2/H2)</f>
         <v>46.296296296296291</v>
       </c>
+      <c r="K2">
+        <v>22</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ref="L2:L17" si="1">K2*J2</f>
+        <v>1018.5185185185184</v>
+      </c>
       <c r="M2">
-        <f t="shared" ref="M2:M17" si="2">L2*K2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+        <f>H2*K2</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>17</v>
       </c>
@@ -768,19 +764,26 @@
       <c r="H3">
         <v>0.5</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3" s="7">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7">
+        <f>100/(D3/H3)</f>
+        <v>98.039215686274503</v>
+      </c>
+      <c r="K3">
+        <v>22</v>
+      </c>
+      <c r="L3">
         <f t="shared" si="1"/>
-        <v>98.039215686274503</v>
+        <v>2156.8627450980389</v>
       </c>
       <c r="M3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+        <f>H3*K3</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
@@ -806,19 +809,26 @@
       <c r="H4">
         <v>0.5</v>
       </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4" s="7">
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="7">
+        <f>100/(D4/H4)</f>
+        <v>54.347826086956516</v>
+      </c>
+      <c r="K4">
+        <v>29</v>
+      </c>
+      <c r="L4">
         <f t="shared" si="1"/>
-        <v>54.347826086956516</v>
+        <v>1576.086956521739</v>
       </c>
       <c r="M4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+        <f>H4*K4</f>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>22</v>
       </c>
@@ -844,18 +854,25 @@
       <c r="H5">
         <v>0.5</v>
       </c>
-      <c r="J5">
-        <v>0.5</v>
-      </c>
-      <c r="K5" s="7">
+      <c r="I5">
+        <v>0.5</v>
+      </c>
+      <c r="J5" s="7">
         <v>0</v>
       </c>
+      <c r="K5">
+        <v>24</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="M5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+        <f>H5*K5</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>20</v>
       </c>
@@ -881,19 +898,26 @@
       <c r="H6">
         <v>0.5</v>
       </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6" s="7">
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="7">
+        <f>100/(D6/H6)</f>
+        <v>58.82352941176471</v>
+      </c>
+      <c r="K6">
+        <v>29</v>
+      </c>
+      <c r="L6">
         <f t="shared" si="1"/>
-        <v>58.82352941176471</v>
+        <v>1705.8823529411766</v>
       </c>
       <c r="M6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+        <f>H6*K6</f>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
@@ -919,22 +943,26 @@
       <c r="H7">
         <v>0.5</v>
       </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7" s="7">
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7">
+        <f>100/(D7/H7)</f>
+        <v>65.78947368421052</v>
+      </c>
+      <c r="K7">
+        <v>32</v>
+      </c>
+      <c r="L7">
         <f t="shared" si="1"/>
-        <v>65.78947368421052</v>
-      </c>
-      <c r="L7">
-        <v>32</v>
+        <v>2105.2631578947367</v>
       </c>
       <c r="M7">
-        <f t="shared" si="2"/>
-        <v>2105.2631578947367</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+        <f>H7*K7</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
@@ -960,22 +988,26 @@
       <c r="H8">
         <v>0.5</v>
       </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8" s="7">
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="7">
+        <f>100/(D8/H8)</f>
+        <v>69.444444444444443</v>
+      </c>
+      <c r="K8">
+        <v>20</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="1"/>
-        <v>69.444444444444443</v>
-      </c>
-      <c r="L8">
-        <v>20</v>
+        <v>1388.8888888888889</v>
       </c>
       <c r="M8">
-        <f t="shared" si="2"/>
-        <v>1388.8888888888889</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+        <f>H8*K8</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>21</v>
       </c>
@@ -1001,18 +1033,25 @@
       <c r="H9">
         <v>0.5</v>
       </c>
-      <c r="J9">
-        <v>0.5</v>
-      </c>
-      <c r="K9" s="7">
+      <c r="I9">
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="7">
         <v>0</v>
       </c>
+      <c r="K9">
+        <v>24</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="M9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+        <f>H9*K9</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>10</v>
       </c>
@@ -1038,22 +1077,26 @@
       <c r="H10">
         <v>0.5</v>
       </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10" s="7">
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" s="7">
+        <f>100/(D10/H10)</f>
+        <v>25.125628140703519</v>
+      </c>
+      <c r="K10">
+        <v>36</v>
+      </c>
+      <c r="L10">
         <f t="shared" si="1"/>
-        <v>25.125628140703519</v>
-      </c>
-      <c r="L10">
-        <v>36</v>
+        <v>904.52261306532671</v>
       </c>
       <c r="M10">
-        <f t="shared" si="2"/>
-        <v>904.52261306532671</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+        <f>H10*K10</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>56</v>
       </c>
@@ -1079,18 +1122,25 @@
       <c r="H11">
         <v>0.5</v>
       </c>
-      <c r="J11">
-        <v>0.5</v>
-      </c>
-      <c r="K11" s="7">
+      <c r="I11">
+        <v>0.5</v>
+      </c>
+      <c r="J11" s="7">
         <v>0</v>
       </c>
+      <c r="K11">
+        <v>24</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="M11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+        <f>H11*K11</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>16</v>
       </c>
@@ -1116,19 +1166,26 @@
       <c r="H12">
         <v>0.5</v>
       </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12" s="7">
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" s="7">
+        <f>100/(D12/H12)</f>
+        <v>25.380710659898476</v>
+      </c>
+      <c r="K12">
+        <v>25</v>
+      </c>
+      <c r="L12">
         <f t="shared" si="1"/>
-        <v>25.380710659898476</v>
+        <v>634.51776649746193</v>
       </c>
       <c r="M12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+        <f>H12*K12</f>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>13</v>
       </c>
@@ -1136,7 +1193,7 @@
         <v>33</v>
       </c>
       <c r="C13">
-        <v>1794</v>
+        <v>1724</v>
       </c>
       <c r="D13" s="1">
         <v>1.25</v>
@@ -1154,22 +1211,26 @@
       <c r="H13">
         <v>0.5</v>
       </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13" s="7">
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13" s="7">
+        <f>100/(D13/H13)</f>
+        <v>40</v>
+      </c>
+      <c r="K13">
+        <v>29</v>
+      </c>
+      <c r="L13">
         <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="L13">
-        <v>29</v>
+        <v>1160</v>
       </c>
       <c r="M13">
-        <f t="shared" si="2"/>
-        <v>1160</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+        <f>H13*K13</f>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>14</v>
       </c>
@@ -1195,19 +1256,26 @@
       <c r="H14">
         <v>0.5</v>
       </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="K14" s="7">
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14" s="7">
+        <f>100/(D14/H14)</f>
+        <v>50.505050505050505</v>
+      </c>
+      <c r="K14">
+        <v>31</v>
+      </c>
+      <c r="L14">
         <f t="shared" si="1"/>
-        <v>50.505050505050505</v>
+        <v>1565.6565656565656</v>
       </c>
       <c r="M14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+        <f>H14*K14</f>
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>9</v>
       </c>
@@ -1233,22 +1301,26 @@
       <c r="H15">
         <v>0.5</v>
       </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="K15" s="7">
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15" s="7">
+        <f>100/(D15/H15)</f>
+        <v>17.361111111111111</v>
+      </c>
+      <c r="K15">
+        <v>20</v>
+      </c>
+      <c r="L15">
         <f t="shared" si="1"/>
-        <v>17.361111111111111</v>
-      </c>
-      <c r="L15">
-        <v>20</v>
+        <v>347.22222222222223</v>
       </c>
       <c r="M15">
-        <f t="shared" si="2"/>
-        <v>347.22222222222223</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+        <f>H15*K15</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>19</v>
       </c>
@@ -1274,16 +1346,23 @@
       <c r="H16">
         <v>0.5</v>
       </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-      <c r="K16" s="7">
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16" s="7">
+        <f>100/(D16/H16)</f>
+        <v>24.390243902439025</v>
+      </c>
+      <c r="K16">
+        <v>16</v>
+      </c>
+      <c r="L16">
         <f t="shared" si="1"/>
-        <v>24.390243902439025</v>
+        <v>390.2439024390244</v>
       </c>
       <c r="M16">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>H16*K16</f>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
@@ -1312,19 +1391,23 @@
       <c r="H17">
         <v>0.5</v>
       </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="K17" s="7">
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17" s="7">
+        <f>100/(D17/H17)</f>
+        <v>19.53125</v>
+      </c>
+      <c r="K17">
+        <v>34</v>
+      </c>
+      <c r="L17">
         <f t="shared" si="1"/>
-        <v>19.53125</v>
-      </c>
-      <c r="L17">
-        <v>34</v>
+        <v>664.0625</v>
       </c>
       <c r="M17">
-        <f t="shared" si="2"/>
-        <v>664.0625</v>
+        <f>H17*K17</f>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
@@ -1353,19 +1436,23 @@
       <c r="H18">
         <v>0.5</v>
       </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
-      <c r="K18" s="7">
-        <f t="shared" si="1"/>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18" s="7">
+        <f>100/(D18/H18)</f>
         <v>16.181229773462785</v>
       </c>
+      <c r="K18">
+        <v>34</v>
+      </c>
       <c r="L18">
-        <v>34</v>
+        <f>K18*J18</f>
+        <v>550.16181229773474</v>
       </c>
       <c r="M18">
-        <f>L18*K18</f>
-        <v>550.16181229773474</v>
+        <f>H18*K18</f>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
@@ -1394,22 +1481,23 @@
       <c r="H19">
         <v>0.5</v>
       </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
-      <c r="K19" s="7">
-        <f t="shared" si="1"/>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19" s="7">
+        <f>100/(D19/H19)</f>
         <v>20.242914979757085</v>
       </c>
+      <c r="K19">
+        <v>30</v>
+      </c>
+      <c r="L19">
+        <f>K19*J19</f>
+        <v>607.28744939271257</v>
+      </c>
       <c r="M19">
-        <f>L19*K19</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="M20" s="15">
-        <f>SUM(M2:M19)</f>
-        <v>7120.1211943689086</v>
+        <f>H19*K19</f>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>